<commit_message>
Add Home page info to content Audit
Updated the information for the Home Page of WRC in the Content
Audit.xlsx
</commit_message>
<xml_diff>
--- a/02 - Content Audit.xlsx
+++ b/02 - Content Audit.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5760" windowWidth="28080" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Content Audit" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>Description</t>
   </si>
@@ -70,9 +70,6 @@
     <t>1 - Very Poor</t>
   </si>
   <si>
-    <t>Home page with features</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>A contact form to contact the company</t>
   </si>
   <si>
-    <t>http://www.vectacorp.com</t>
-  </si>
-  <si>
     <t>http://www.vectacorp.com/aboutus.html</t>
   </si>
   <si>
@@ -124,13 +118,27 @@
     <t>Action</t>
   </si>
   <si>
-    <t>Keep as is</t>
-  </si>
-  <si>
     <t>Improve</t>
   </si>
   <si>
     <t>Consolidate</t>
+  </si>
+  <si>
+    <t>3 - Poor</t>
+  </si>
+  <si>
+    <t>5 - Poor</t>
+  </si>
+  <si>
+    <t>http://www.wrcsd.org</t>
+  </si>
+  <si>
+    <t>Landing page for WRC with Navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missing current events and activities in a manner that’s engaging to its audience.  
+Needs ability to receive help in a more direct and obvious way, currently getting help doesn’t appear to be the focus of the homepage
+</t>
   </si>
 </sst>
 </file>
@@ -216,8 +224,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -324,7 +334,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -366,6 +376,7 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -407,6 +418,7 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -743,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -790,49 +802,51 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" s="7" customFormat="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="7" customFormat="1" ht="234">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="10"/>
+        <v>13</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="K2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="Y2" s="9" t="s">
         <v>10</v>
@@ -840,10 +854,10 @@
     </row>
     <row r="3" spans="1:25" s="7" customFormat="1" ht="126">
       <c r="A3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>11</v>
@@ -851,8 +865,8 @@
       <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>13</v>
+      <c r="E3" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>10</v>
@@ -867,13 +881,13 @@
         <v>10</v>
       </c>
       <c r="J3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="L3" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y3" s="9" t="s">
         <v>11</v>
@@ -881,10 +895,10 @@
     </row>
     <row r="4" spans="1:25" s="7" customFormat="1">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>11</v>
@@ -892,8 +906,8 @@
       <c r="D4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>11</v>
+      <c r="E4" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>11</v>
@@ -909,10 +923,10 @@
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Y4" s="9" t="s">
         <v>13</v>
@@ -920,10 +934,10 @@
     </row>
     <row r="5" spans="1:25" s="7" customFormat="1">
       <c r="A5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>13</v>
@@ -931,8 +945,8 @@
       <c r="D5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>13</v>
+      <c r="E5" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>13</v>
@@ -948,10 +962,10 @@
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Y5" s="9" t="s">
         <v>12</v>
@@ -959,10 +973,10 @@
     </row>
     <row r="6" spans="1:25" s="7" customFormat="1">
       <c r="A6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>12</v>
@@ -987,10 +1001,10 @@
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Y6" s="9" t="s">
         <v>14</v>
@@ -1054,7 +1068,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C21:C1048576 C2:D6 F19:F1048576 G16:G1048576 H11:H1048576 E7:E1048576 I10:I1048576 F2:I5 E6:I6</xm:sqref>
+          <xm:sqref>C21:C1048576 F19:F1048576 G16:G1048576 H11:H1048576 E7:E1048576 I10:I1048576 C2:I6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>